<commit_message>
xlsx reader test - ok
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/office.xlsx
+++ b/src/test/resources/xlsx/office.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyProjects\apas\src\test\resources\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Java\MyProjects\apas\src\test\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CC164D-EAE5-46E2-82CE-4324CF4C2DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD447291-F983-42F7-AA27-1ECAB753E700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{317C8D59-AC1D-4C59-8E88-2BFC1F6C91AC}"/>
+    <workbookView xWindow="630" yWindow="3600" windowWidth="21600" windowHeight="11385" xr2:uid="{317C8D59-AC1D-4C59-8E88-2BFC1F6C91AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,26 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>INPUT:officeData,TYPE:initial</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>officeTypeCode</t>
-  </si>
-  <si>
-    <t>parentOfficeCode</t>
-  </si>
-  <si>
     <t>231101</t>
   </si>
   <si>
@@ -71,6 +56,18 @@
   </si>
   <si>
     <t>231000</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>OfficeTypeCode</t>
+  </si>
+  <si>
+    <t>ParentOfficeCode</t>
   </si>
 </sst>
 </file>
@@ -423,73 +420,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C46DA92-79CC-4F24-A91E-23C9D7AA46E6}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>